<commit_message>
end to end complete test
</commit_message>
<xml_diff>
--- a/iGEM_LUDOX_OD_calibration_2018.xlsx
+++ b/iGEM_LUDOX_OD_calibration_2018.xlsx
@@ -140,10 +140,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -153,11 +154,19 @@
     <xf numFmtId="14" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
+      <protection locked="0" hidden="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -233,6 +242,61 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/comments/comment1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>PAML autogeneration, do not modify</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <t>https://bbn.com/scratch/iGEM_LUDOX_OD_calibration_2018</t>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0">
+      <text>
+        <t>https://bbn.com/scratch/iGEM_LUDOX_OD_calibration_2018/Container1_A2 https://bbn.com/scratch/ddH2O</t>
+      </text>
+    </comment>
+    <comment ref="E10" authorId="0" shapeId="0">
+      <text>
+        <t>https://bbn.com/scratch/iGEM_LUDOX_OD_calibration_2018/Container1_A1 https://bbn.com/scratch/LUDOX</t>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0">
+      <text>
+        <t>https://bbn.com/scratch/iGEM_LUDOX_OD_calibration_2018/Container1_B2 https://bbn.com/scratch/ddH2O</t>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="0" shapeId="0">
+      <text>
+        <t>https://bbn.com/scratch/iGEM_LUDOX_OD_calibration_2018/Container1_B1 https://bbn.com/scratch/LUDOX</t>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0">
+      <text>
+        <t>https://bbn.com/scratch/iGEM_LUDOX_OD_calibration_2018/Container1_C2 https://bbn.com/scratch/ddH2O</t>
+      </text>
+    </comment>
+    <comment ref="E12" authorId="0" shapeId="0">
+      <text>
+        <t>https://bbn.com/scratch/iGEM_LUDOX_OD_calibration_2018/Container1_C1 https://bbn.com/scratch/LUDOX</t>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0" shapeId="0">
+      <text>
+        <t>https://bbn.com/scratch/iGEM_LUDOX_OD_calibration_2018/Container1_D2 https://bbn.com/scratch/ddH2O</t>
+      </text>
+    </comment>
+    <comment ref="E13" authorId="0" shapeId="0">
+      <text>
+        <t>https://bbn.com/scratch/iGEM_LUDOX_OD_calibration_2018/Container1_D1 https://bbn.com/scratch/LUDOX</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -531,7 +595,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -539,7 +603,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -553,53 +617,53 @@
           <t>Protocol Execution Record:</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>iGEM 2018 LUDOX OD calibration protocol</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Person Executing</t>
         </is>
       </c>
       <c r="B2" s="7" t="n"/>
-      <c r="C2" s="4" t="n"/>
+      <c r="C2" s="8" t="n"/>
       <c r="D2" s="7" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>Date Executed</t>
         </is>
       </c>
       <c r="B3" s="7" t="n"/>
-      <c r="C3" s="4" t="n"/>
+      <c r="C3" s="8" t="n"/>
       <c r="D3" s="7" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="inlineStr">
+      <c r="A4" s="4" t="inlineStr">
         <is>
           <t>Date Reported</t>
         </is>
       </c>
       <c r="B4" s="7" t="n"/>
-      <c r="C4" s="5" t="n"/>
+      <c r="C4" s="9" t="n"/>
       <c r="D4" s="7" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Blue = Do not change; Green = free text</t>
+          <t>Green cells are entry locations. Any text outside these locations will be ignored</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>Report from Step 3</t>
+          <t>Report from Step 4</t>
         </is>
       </c>
     </row>
@@ -616,74 +680,75 @@
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="8" t="inlineStr">
+      <c r="B9" s="10" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E9" s="8" t="inlineStr">
+      <c r="E9" s="10" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="8" t="inlineStr">
+      <c r="A10" s="10" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="B10" s="9" t="n"/>
-      <c r="D10" s="8" t="inlineStr">
+      <c r="B10" s="11" t="n"/>
+      <c r="D10" s="10" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="E10" s="9" t="n"/>
+      <c r="E10" s="11" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="8" t="inlineStr">
+      <c r="A11" s="10" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="B11" s="9" t="n"/>
-      <c r="D11" s="8" t="inlineStr">
+      <c r="B11" s="11" t="n"/>
+      <c r="D11" s="10" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="E11" s="9" t="n"/>
+      <c r="E11" s="11" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="8" t="inlineStr">
+      <c r="A12" s="10" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="B12" s="9" t="n"/>
-      <c r="D12" s="8" t="inlineStr">
+      <c r="B12" s="11" t="n"/>
+      <c r="D12" s="10" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="E12" s="9" t="n"/>
+      <c r="E12" s="11" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="8" t="inlineStr">
+      <c r="A13" s="10" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
-      <c r="B13" s="9" t="n"/>
-      <c r="D13" s="8" t="inlineStr">
+      <c r="B13" s="11" t="n"/>
+      <c r="D13" s="10" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
-      <c r="E13" s="9" t="n"/>
+      <c r="E13" s="11" t="n"/>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1"/>
   <mergeCells count="6">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -693,5 +758,6 @@
     <mergeCell ref="C4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>